<commit_message>
se agregan nuevas casetas
</commit_message>
<xml_diff>
--- a/data/casetas.xlsx
+++ b/data/casetas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonvc/NODE LOCAL/bot-casetas-mexico/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonvc/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C23C77-3763-344C-9BE9-47573C1D895B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B164EDAC-C03F-7641-9328-A011FB86129C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12040" yWindow="5420" windowWidth="19300" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casetas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="52">
   <si>
     <t>Nombre</t>
   </si>
@@ -62,13 +62,127 @@
   </si>
   <si>
     <t>Caseta San Juan del Río</t>
+  </si>
+  <si>
+    <t>Caseta chalco</t>
+  </si>
+  <si>
+    <t>Mexico-puebla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caseta san marcos bis </t>
+  </si>
+  <si>
+    <t>Caseta san martin Texmelucan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caseta san marcos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseta tehuacan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseta amozoc </t>
+  </si>
+  <si>
+    <t>circuito ext mexiquense</t>
+  </si>
+  <si>
+    <t>caseta T1 Tultepec</t>
+  </si>
+  <si>
+    <t>caseta T0 Jorobas</t>
+  </si>
+  <si>
+    <t>caseta T2 Conmex</t>
+  </si>
+  <si>
+    <t>caseta T3 Nabor Carrillo (Puebla)</t>
+  </si>
+  <si>
+    <t>casetas T3 nabor carrillo (Bordo)</t>
+  </si>
+  <si>
+    <t>caseta T4 chalco</t>
+  </si>
+  <si>
+    <t>caseta A2 hank gonzalez</t>
+  </si>
+  <si>
+    <t>caseta A6 periferico</t>
+  </si>
+  <si>
+    <t>caseta A21 bordo de xochiaca</t>
+  </si>
+  <si>
+    <t>casetas A22 bordo de xochiaca</t>
+  </si>
+  <si>
+    <t>caseta T7 texcoco</t>
+  </si>
+  <si>
+    <t>caseta A27 san buena ventura</t>
+  </si>
+  <si>
+    <t>caseta A28 san buena ventura</t>
+  </si>
+  <si>
+    <t>caseta T5 tultitlan</t>
+  </si>
+  <si>
+    <t>caseta T6 cucutitlan</t>
+  </si>
+  <si>
+    <t>caseta san cristobal (ecatepec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseta revolucion 91 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseta ojo de agua </t>
+  </si>
+  <si>
+    <t>mexico-pachuca</t>
+  </si>
+  <si>
+    <t>caseta peñon texcoco</t>
+  </si>
+  <si>
+    <t>peñon-texcoco</t>
+  </si>
+  <si>
+    <t>casetas entronque peñon</t>
+  </si>
+  <si>
+    <t>caseta de tlalpan</t>
+  </si>
+  <si>
+    <t>mexico-cuernavaca</t>
+  </si>
+  <si>
+    <t>caseta tres marias</t>
+  </si>
+  <si>
+    <t>caseta la venta-atizapan</t>
+  </si>
+  <si>
+    <t>toluca-naucalpan</t>
+  </si>
+  <si>
+    <t>caseta marquesa</t>
+  </si>
+  <si>
+    <t>mexico-toluca</t>
+  </si>
+  <si>
+    <t>caseta la venta-marquesa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -81,6 +195,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -108,9 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,11 +566,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -567,7 +697,936 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>-98.881674000000004</v>
+      </c>
+      <c r="C5">
+        <v>19.291975999999998</v>
+      </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>43</v>
+      </c>
+      <c r="F5">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>-98.875939000000002</v>
+      </c>
+      <c r="C6">
+        <v>19.293316999999998</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>43</v>
+      </c>
+      <c r="F6">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>-98.385598999999999</v>
+      </c>
+      <c r="C7">
+        <v>19.240756999999999</v>
+      </c>
+      <c r="D7">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <v>111</v>
+      </c>
+      <c r="F7">
+        <v>119</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>-98.870662999999993</v>
+      </c>
+      <c r="C8">
+        <v>19.296441999999999</v>
+      </c>
+      <c r="D8">
+        <v>156</v>
+      </c>
+      <c r="E8">
+        <v>288</v>
+      </c>
+      <c r="F8">
+        <v>301</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>-97.456113999999999</v>
+      </c>
+      <c r="C9">
+        <v>18.487238000000001</v>
+      </c>
+      <c r="D9">
+        <v>52</v>
+      </c>
+      <c r="E9">
+        <v>118</v>
+      </c>
+      <c r="F9">
+        <v>119</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>-98.032128999999998</v>
+      </c>
+      <c r="C10" s="2">
+        <v>19.050028999999999</v>
+      </c>
+      <c r="D10">
+        <v>84</v>
+      </c>
+      <c r="E10">
+        <v>162</v>
+      </c>
+      <c r="F10">
+        <v>170</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>-99.239707999999993</v>
+      </c>
+      <c r="C11">
+        <v>19.819889</v>
+      </c>
+      <c r="D11">
+        <v>155</v>
+      </c>
+      <c r="E11">
+        <v>321</v>
+      </c>
+      <c r="F11">
+        <v>322</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>-99.079931999999999</v>
+      </c>
+      <c r="C12">
+        <v>19.694092999999999</v>
+      </c>
+      <c r="D12">
+        <v>109</v>
+      </c>
+      <c r="E12">
+        <v>248</v>
+      </c>
+      <c r="F12">
+        <v>248</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>-99.020345000000006</v>
+      </c>
+      <c r="C13">
+        <v>19.575541999999999</v>
+      </c>
+      <c r="D13">
+        <v>77</v>
+      </c>
+      <c r="E13">
+        <v>177</v>
+      </c>
+      <c r="F13">
+        <v>177</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>-98.998236000000006</v>
+      </c>
+      <c r="C14">
+        <v>19.435749000000001</v>
+      </c>
+      <c r="D14">
+        <v>48</v>
+      </c>
+      <c r="E14">
+        <v>111</v>
+      </c>
+      <c r="F14">
+        <v>111</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>-98.998656999999994</v>
+      </c>
+      <c r="C15">
+        <v>19.435922999999999</v>
+      </c>
+      <c r="D15">
+        <v>34</v>
+      </c>
+      <c r="E15">
+        <v>77</v>
+      </c>
+      <c r="F15">
+        <v>77</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>-98.875102999999996</v>
+      </c>
+      <c r="C16">
+        <v>19.300114000000001</v>
+      </c>
+      <c r="D16">
+        <v>112</v>
+      </c>
+      <c r="E16">
+        <v>256</v>
+      </c>
+      <c r="F16">
+        <v>256</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>-99.038515000000004</v>
+      </c>
+      <c r="C17">
+        <v>19.610797000000002</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>46</v>
+      </c>
+      <c r="F17">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>-99.016385999999997</v>
+      </c>
+      <c r="C18">
+        <v>19.487165000000001</v>
+      </c>
+      <c r="D18">
+        <v>26</v>
+      </c>
+      <c r="E18">
+        <v>60</v>
+      </c>
+      <c r="F18">
+        <v>60</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>-98.998570999999998</v>
+      </c>
+      <c r="C19">
+        <v>19.425533000000001</v>
+      </c>
+      <c r="D19">
+        <v>32</v>
+      </c>
+      <c r="E19">
+        <v>73</v>
+      </c>
+      <c r="F19">
+        <v>73</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>-98.998734999999996</v>
+      </c>
+      <c r="C20">
+        <v>19.425757999999998</v>
+      </c>
+      <c r="D20">
+        <v>32</v>
+      </c>
+      <c r="E20">
+        <v>73</v>
+      </c>
+      <c r="F20">
+        <v>73</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>-98.910869000000005</v>
+      </c>
+      <c r="C21">
+        <v>19.450638999999999</v>
+      </c>
+      <c r="D21">
+        <v>47</v>
+      </c>
+      <c r="E21">
+        <v>108</v>
+      </c>
+      <c r="F21">
+        <v>108</v>
+      </c>
+      <c r="G21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>-98.871780000000001</v>
+      </c>
+      <c r="C22">
+        <v>19.307054999999998</v>
+      </c>
+      <c r="D22">
+        <v>104</v>
+      </c>
+      <c r="E22">
+        <v>238</v>
+      </c>
+      <c r="F22">
+        <v>238</v>
+      </c>
+      <c r="G22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>-98.875044000000003</v>
+      </c>
+      <c r="C23">
+        <v>19.299982</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>26</v>
+      </c>
+      <c r="F23">
+        <v>26</v>
+      </c>
+      <c r="G23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>-99.164170999999996</v>
+      </c>
+      <c r="C24">
+        <v>19.637958999999999</v>
+      </c>
+      <c r="D24">
+        <v>40</v>
+      </c>
+      <c r="E24">
+        <v>91</v>
+      </c>
+      <c r="F24">
+        <v>91</v>
+      </c>
+      <c r="G24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25">
+        <v>-99.205059000000006</v>
+      </c>
+      <c r="C25">
+        <v>19.635532000000001</v>
+      </c>
+      <c r="D25">
+        <v>29</v>
+      </c>
+      <c r="E25">
+        <v>66</v>
+      </c>
+      <c r="F25">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>-99.041917999999995</v>
+      </c>
+      <c r="C26">
+        <v>19.587889000000001</v>
+      </c>
+      <c r="D26">
+        <v>26</v>
+      </c>
+      <c r="E26">
+        <v>44</v>
+      </c>
+      <c r="F26">
+        <v>44</v>
+      </c>
+      <c r="G26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27">
+        <v>-99.037999999999997</v>
+      </c>
+      <c r="C27">
+        <v>19.602851999999999</v>
+      </c>
+      <c r="D27">
+        <v>41</v>
+      </c>
+      <c r="E27">
+        <v>75</v>
+      </c>
+      <c r="F27">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28">
+        <v>-99.029195000000001</v>
+      </c>
+      <c r="C28">
+        <v>19.618784999999999</v>
+      </c>
+      <c r="D28">
+        <v>65</v>
+      </c>
+      <c r="E28">
+        <v>129</v>
+      </c>
+      <c r="F28">
+        <v>129</v>
+      </c>
+      <c r="G28" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>-99.033747000000005</v>
+      </c>
+      <c r="C29">
+        <v>19.458393000000001</v>
+      </c>
+      <c r="D29">
+        <v>55</v>
+      </c>
+      <c r="E29">
+        <v>110</v>
+      </c>
+      <c r="F29">
+        <v>110</v>
+      </c>
+      <c r="G29" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>-98.912721000000005</v>
+      </c>
+      <c r="C30">
+        <v>19.502880000000001</v>
+      </c>
+      <c r="D30">
+        <v>55</v>
+      </c>
+      <c r="E30">
+        <v>110</v>
+      </c>
+      <c r="F30">
+        <v>110</v>
+      </c>
+      <c r="G30" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>-99.004378000000003</v>
+      </c>
+      <c r="C31">
+        <v>19.468900000000001</v>
+      </c>
+      <c r="D31">
+        <v>41</v>
+      </c>
+      <c r="E31">
+        <v>85</v>
+      </c>
+      <c r="F31">
+        <v>85</v>
+      </c>
+      <c r="G31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <v>-99.148836000000003</v>
+      </c>
+      <c r="C32">
+        <v>19.242341</v>
+      </c>
+      <c r="D32">
+        <v>136</v>
+      </c>
+      <c r="E32">
+        <v>250</v>
+      </c>
+      <c r="F32">
+        <v>252</v>
+      </c>
+      <c r="G32" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <v>-99.240983999999997</v>
+      </c>
+      <c r="C33">
+        <v>19.05631</v>
+      </c>
+      <c r="D33">
+        <v>51</v>
+      </c>
+      <c r="E33">
+        <v>11</v>
+      </c>
+      <c r="F33">
+        <v>114</v>
+      </c>
+      <c r="G33" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34">
+        <v>-99.296637000000004</v>
+      </c>
+      <c r="C34">
+        <v>19.431676</v>
+      </c>
+      <c r="D34">
+        <v>144</v>
+      </c>
+      <c r="E34">
+        <v>262</v>
+      </c>
+      <c r="F34">
+        <v>415</v>
+      </c>
+      <c r="G34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>-99.314075000000003</v>
+      </c>
+      <c r="C35">
+        <v>19.332788000000001</v>
+      </c>
+      <c r="D35">
+        <v>105</v>
+      </c>
+      <c r="E35">
+        <v>210</v>
+      </c>
+      <c r="F35">
+        <v>210</v>
+      </c>
+      <c r="G35" t="s">
+        <v>50</v>
+      </c>
+      <c r="H35" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36">
+        <v>-99.315567000000001</v>
+      </c>
+      <c r="C36">
+        <v>19.330030000000001</v>
+      </c>
+      <c r="D36">
+        <v>52</v>
+      </c>
+      <c r="E36">
+        <v>105</v>
+      </c>
+      <c r="F36">
+        <v>105</v>
+      </c>
+      <c r="G36" t="s">
+        <v>50</v>
+      </c>
+      <c r="H36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mejora radio a 5 metros de distancia de las casetas funcionando
</commit_message>
<xml_diff>
--- a/data/casetas.xlsx
+++ b/data/casetas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonvc/NODE LOCAL/bot-casetas-mexico/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhonvc/NODE LOCAL/BOT-CASETAS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DE699D-034D-1744-81E6-0AAD67A42EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BC8AA2-F5A7-6E41-BCBC-D19AE1AD6B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12040" yWindow="5420" windowWidth="19300" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="53">
   <si>
     <t>Nombre</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>caseta la venta-marquesa</t>
+  </si>
+  <si>
+    <t>S-N</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -636,7 +641,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -644,10 +649,10 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>-99.212200999999993</v>
+        <v>-99.212456000000003</v>
       </c>
       <c r="C3">
-        <v>19.743611999999999</v>
+        <v>19.743592</v>
       </c>
       <c r="D3">
         <v>150</v>
@@ -665,7 +670,7 @@
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -694,7 +699,7 @@
         <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -789,10 +794,10 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>-98.870662999999993</v>
+        <v>-98.870620000000002</v>
       </c>
       <c r="C8">
-        <v>19.296441999999999</v>
+        <v>19.296437000000001</v>
       </c>
       <c r="D8">
         <v>156</v>

</xml_diff>